<commit_message>
actualizacion 9 de Abril, se tuvo que volver a cargar el informe mensual de marzo
</commit_message>
<xml_diff>
--- a/Resultado/informe_mensual_marzo_2025.xlsx
+++ b/Resultado/informe_mensual_marzo_2025.xlsx
@@ -91,16 +91,16 @@
     <t>1.46%</t>
   </si>
   <si>
-    <t>25.29%</t>
-  </si>
-  <si>
-    <t>22.83%</t>
-  </si>
-  <si>
-    <t>26.25%</t>
-  </si>
-  <si>
-    <t>7.92%</t>
+    <t>25.31%</t>
+  </si>
+  <si>
+    <t>22.76%</t>
+  </si>
+  <si>
+    <t>25.83%</t>
+  </si>
+  <si>
+    <t>8.33%</t>
   </si>
   <si>
     <t>4.80</t>
@@ -109,34 +109,34 @@
     <t>82.25%</t>
   </si>
   <si>
-    <t>7,612,035,035,395</t>
-  </si>
-  <si>
-    <t>1.12%</t>
-  </si>
-  <si>
-    <t>29.61%</t>
+    <t>7,312,851,083,792</t>
+  </si>
+  <si>
+    <t>1.11%</t>
+  </si>
+  <si>
+    <t>29.62%</t>
   </si>
   <si>
     <t>22.25%</t>
   </si>
   <si>
-    <t>55.83%</t>
-  </si>
-  <si>
-    <t>10.0%</t>
-  </si>
-  <si>
-    <t>8,677,504,600,371</t>
+    <t>56.25%</t>
+  </si>
+  <si>
+    <t>9.58%</t>
+  </si>
+  <si>
+    <t>8,332,918,568,409</t>
   </si>
   <si>
     <t>1.95%</t>
   </si>
   <si>
-    <t>54.91%</t>
-  </si>
-  <si>
-    <t>45.09%</t>
+    <t>54.97%</t>
+  </si>
+  <si>
+    <t>45.03%</t>
   </si>
   <si>
     <t>82.08%</t>
@@ -145,7 +145,7 @@
     <t>17.92%</t>
   </si>
   <si>
-    <t>16,289,539,635,766</t>
+    <t>15,645,769,652,201</t>
   </si>
 </sst>
 </file>
@@ -528,13 +528,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>8310</v>
+        <v>8288</v>
       </c>
       <c r="C2">
-        <v>8729</v>
+        <v>8709</v>
       </c>
       <c r="D2">
-        <v>17040</v>
+        <v>16997</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -556,13 +556,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C4">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D4">
-        <v>363</v>
+        <v>347</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -570,13 +570,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C5">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D5">
-        <v>148</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -584,13 +584,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C6">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D6">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -598,13 +598,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -682,10 +682,10 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D13">
         <v>197</v>
@@ -696,10 +696,10 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C14">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14">
         <v>43</v>
@@ -780,13 +780,13 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>22112036</v>
+        <v>21251053</v>
       </c>
       <c r="C20">
-        <v>25934114</v>
+        <v>24924103</v>
       </c>
       <c r="D20">
-        <v>48046150</v>
+        <v>46175156</v>
       </c>
     </row>
     <row r="21" spans="1:4">

</xml_diff>